<commit_message>
prepared species richness and shannon's data for analysis
</commit_message>
<xml_diff>
--- a/00_Data/Master_files/plant_info_MASTER.xlsx
+++ b/00_Data/Master_files/plant_info_MASTER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annabelsmith/Documents/00_UQ_offline/STJW_analysis/00_Data/Master_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186E9DF4-752C-834B-817D-1FA08F1CE30B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E034FE3-CD5E-3645-BE58-18102C0BC610}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="566">
   <si>
     <t>Species</t>
   </si>
@@ -1701,6 +1701,36 @@
   </si>
   <si>
     <t>Era_sp.</t>
+  </si>
+  <si>
+    <t>PLANT INFO NOTES:</t>
+  </si>
+  <si>
+    <t>COUNT DATA NOTES:</t>
+  </si>
+  <si>
+    <t>DATA ORGANISATION:</t>
+  </si>
+  <si>
+    <t>There's only one species that's listed as "Rare" ("Zornia dyctocarpa") so we won't be using this column in the analysis; leave as is.</t>
+  </si>
+  <si>
+    <t>The indicator variable only had one level "1", so I have replaced the NAs with zero. This makes it easier to work with as a simple, yes==1; no==0 binary variable.</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Boom spray - fine droplet</t>
+  </si>
+  <si>
+    <t>Spot spray</t>
   </si>
 </sst>
 </file>
@@ -2616,10 +2646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A07B7B-DA92-6046-97FE-19EF85E12869}">
-  <dimension ref="A3:A48"/>
+  <dimension ref="A3:A55"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2638,186 +2668,211 @@
     <row r="4" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="12"/>
     </row>
-    <row r="5" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="10" t="s">
-        <v>514</v>
+    <row r="5" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="11" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="6" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="7" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10" t="s">
-        <v>529</v>
+        <v>515</v>
       </c>
     </row>
     <row r="8" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
-        <v>516</v>
+        <v>529</v>
       </c>
     </row>
     <row r="9" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="10" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="10" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="10" t="s">
-        <v>517</v>
-      </c>
-    </row>
+    <row r="11" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="12" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="13" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="10" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="14" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="10" t="s">
-        <v>519</v>
-      </c>
-    </row>
+    <row r="15" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="16" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A16" s="10" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="17" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A17" s="10" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="10" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="19" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="13" t="s">
-        <v>531</v>
-      </c>
-    </row>
+    <row r="19" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="20" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="21" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="13" t="s">
-        <v>551</v>
+        <v>532</v>
       </c>
     </row>
     <row r="22" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="13" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="13" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="23" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="24" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="13" t="s">
-        <v>534</v>
-      </c>
-    </row>
+    <row r="24" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="25" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A25" s="13" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
     </row>
     <row r="26" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A26" s="13" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="13" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="27" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="28" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="10" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="10" t="s">
-        <v>509</v>
+    <row r="28" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="29" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="11" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="30" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A30" s="10" t="s">
-        <v>510</v>
+        <v>536</v>
       </c>
     </row>
     <row r="31" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A31" s="10" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+        <v>509</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="10" t="s">
+        <v>510</v>
+      </c>
+    </row>
     <row r="33" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A33" s="10" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="35" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="10" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="34" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="10" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="36" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A36" s="10" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="10" t="s">
-        <v>522</v>
-      </c>
-    </row>
+        <v>513</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="38" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A38" s="10" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="39" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A39" s="10" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+        <v>522</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="10" t="s">
+        <v>523</v>
+      </c>
+    </row>
     <row r="41" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A41" s="10" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="42" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="43" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A43" s="10" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="45" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="10" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="44" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="10" t="s">
+    <row r="46" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="10" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="45" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="10" t="s">
+    <row r="47" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="10" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="46" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="10"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="10"/>
+    </row>
+    <row r="49" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="11" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A50" s="1" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A48" s="1" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A51" s="1" t="s">
         <v>554</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A53" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A55" s="1" t="s">
+        <v>559</v>
       </c>
     </row>
   </sheetData>
@@ -2827,10 +2882,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D230"/>
+  <dimension ref="A2:D234"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2843,1297 +2898,1329 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>549</v>
+        <v>561</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>548</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>550</v>
+        <v>562</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>540</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>547</v>
+        <v>565</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>542</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="C4" s="1">
-        <v>35</v>
+        <v>564</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C9" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C10" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C11" s="1">
         <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>548</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>489</v>
+        <v>545</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="1">
-        <v>20</v>
+        <v>546</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="C15" s="1">
-        <v>30</v>
+      <c r="A15" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1">
-        <v>40</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>496</v>
+        <v>12</v>
       </c>
       <c r="C17" s="1">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>498</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="C19" s="1">
-        <v>70</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>502</v>
+        <v>19</v>
       </c>
       <c r="C20" s="1">
-        <v>80</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="C21" s="1">
-        <v>90</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="C22" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C23" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="C24" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="C25" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C26" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="3" t="s">
+    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="2" t="s">
+    <row r="30" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>271</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A28" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A29" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A30" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>281</v>
+        <v>273</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="2"/>
+      <c r="A33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="3"/>
-      <c r="D34" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A38" s="3"/>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A39" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>476</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="6" t="s">
-        <v>400</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="6" t="s">
-        <v>26</v>
+        <v>400</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="D41" s="5">
-        <v>310</v>
+        <v>15</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="6" t="s">
-        <v>402</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="D42" s="5">
-        <v>195</v>
+        <v>401</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="6" t="s">
-        <v>403</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="D43" s="5">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>479</v>
-      </c>
-      <c r="D44" s="5">
-        <f>D41-D42+D43</f>
-        <v>118</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" s="6" t="s">
-        <v>404</v>
+        <v>27</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="D45" s="5">
+        <v>310</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" s="6" t="s">
-        <v>405</v>
+        <v>402</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="D46" s="5">
+        <v>195</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" s="6" t="s">
-        <v>30</v>
+        <v>403</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="D47" s="5">
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="D48" s="5">
+        <f>D45-D46+D47</f>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A49" s="6" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A50" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A51" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A52" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A53" s="6" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A54" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A55" s="6" t="s">
         <v>408</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A52" s="7" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A53" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A54" s="7" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A55" s="7" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A56" s="7" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A57" s="7" t="s">
-        <v>412</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A58" s="7" t="s">
-        <v>45</v>
+        <v>410</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A59" s="7" t="s">
-        <v>413</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A60" s="7" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A61" s="7" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A62" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A63" s="7" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A64" s="7" t="s">
-        <v>51</v>
+        <v>414</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A65" s="7" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A66" s="7" t="s">
-        <v>418</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A67" s="7" t="s">
-        <v>59</v>
+        <v>416</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A68" s="7" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A69" s="7" t="s">
-        <v>62</v>
+        <v>417</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A70" s="7" t="s">
-        <v>64</v>
+        <v>418</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A71" s="7" t="s">
-        <v>419</v>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A72" s="7" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A73" s="7" t="s">
-        <v>420</v>
+        <v>62</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A74" s="7" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A75" s="7" t="s">
-        <v>73</v>
+        <v>419</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A76" s="7" t="s">
-        <v>421</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A77" s="7" t="s">
-        <v>75</v>
+        <v>420</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A78" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A79" s="7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A80" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A81" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A82" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A83" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A84" s="7" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A85" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A86" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A87" s="7" t="s">
         <v>423</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A84" s="6" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A85" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A86" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A87" s="6" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A88" s="6" t="s">
-        <v>87</v>
+        <v>424</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A89" s="6" t="s">
-        <v>426</v>
+        <v>83</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A90" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A91" s="6" t="s">
-        <v>89</v>
+        <v>425</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A92" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A93" s="6" t="s">
-        <v>91</v>
+        <v>426</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A94" s="6" t="s">
-        <v>427</v>
+        <v>88</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A95" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A96" s="6" t="s">
-        <v>428</v>
+        <v>90</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A97" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A98" s="6" t="s">
-        <v>94</v>
+        <v>427</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A99" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A100" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A101" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A102" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A103" s="6" t="s">
-        <v>430</v>
+        <v>95</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A104" s="6" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A105" s="6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A106" s="6" t="s">
-        <v>432</v>
+        <v>98</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A107" s="6" t="s">
-        <v>101</v>
+        <v>430</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A108" s="6" t="s">
-        <v>102</v>
+        <v>431</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A109" s="6" t="s">
-        <v>433</v>
+        <v>100</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A110" s="6" t="s">
-        <v>103</v>
+        <v>432</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A111" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A112" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A113" s="6" t="s">
-        <v>110</v>
+        <v>433</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A114" s="6" t="s">
-        <v>434</v>
+        <v>103</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A115" s="6" t="s">
-        <v>435</v>
+        <v>105</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A116" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A117" s="6" t="s">
-        <v>436</v>
+        <v>110</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A118" s="6" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A119" s="6" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A120" s="6" t="s">
-        <v>439</v>
+        <v>112</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A121" s="6" t="s">
-        <v>121</v>
+        <v>436</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A122" s="6" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A123" s="6" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A124" s="6" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A125" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A126" s="6" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A127" s="6" t="s">
-        <v>124</v>
+        <v>441</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A128" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A129" s="6" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A130" s="6" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A131" s="6" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A132" s="6" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A133" s="6" t="s">
-        <v>447</v>
+        <v>129</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A134" s="6" t="s">
-        <v>131</v>
+        <v>445</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A135" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A136" s="6" t="s">
-        <v>133</v>
+        <v>446</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A137" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" ht="15" x14ac:dyDescent="0.15">
-      <c r="A138" s="8" t="s">
-        <v>137</v>
+        <v>447</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A138" s="6" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A139" s="6" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A140" s="6" t="s">
-        <v>448</v>
+        <v>133</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A141" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A142" s="6" t="s">
-        <v>139</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A142" s="8" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A143" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A144" s="6" t="s">
-        <v>142</v>
+        <v>448</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A145" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A146" s="6" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A147" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A148" s="6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A149" s="6" t="s">
-        <v>449</v>
+        <v>143</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A150" s="6" t="s">
-        <v>450</v>
+        <v>145</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A151" s="6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A152" s="6" t="s">
-        <v>451</v>
+        <v>148</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A153" s="6" t="s">
-        <v>154</v>
+        <v>449</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A154" s="6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A155" s="6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A156" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A157" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A158" s="6" t="s">
-        <v>159</v>
+        <v>452</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A159" s="6" t="s">
-        <v>454</v>
+        <v>156</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A160" s="6" t="s">
-        <v>160</v>
+        <v>453</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A161" s="6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A162" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A163" s="6" t="s">
-        <v>164</v>
+        <v>454</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A164" s="6" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A165" s="6" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A166" s="6" t="s">
-        <v>455</v>
+        <v>162</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A167" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A168" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A169" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A170" s="6" t="s">
-        <v>173</v>
+        <v>455</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A171" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A172" s="6" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A173" s="6" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A174" s="6" t="s">
-        <v>456</v>
+        <v>173</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A175" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A176" s="6" t="s">
-        <v>457</v>
+        <v>175</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A177" s="6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A178" s="6" t="s">
-        <v>183</v>
+        <v>456</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A179" s="6" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A180" s="6" t="s">
-        <v>185</v>
+        <v>457</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A181" s="6" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A182" s="6" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A183" s="6" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A184" s="6" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A185" s="6" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A186" s="6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A187" s="6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A188" s="6" t="s">
-        <v>458</v>
+        <v>191</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A189" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A190" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A191" s="6" t="s">
-        <v>459</v>
+        <v>194</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A192" s="6" t="s">
-        <v>198</v>
+        <v>458</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A193" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A194" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A195" s="6" t="s">
-        <v>204</v>
+        <v>459</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A196" s="6" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A197" s="6" t="s">
-        <v>460</v>
+        <v>199</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A198" s="6" t="s">
-        <v>461</v>
+        <v>200</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A199" s="6" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A200" s="6" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A201" s="6" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A202" s="6" t="s">
-        <v>214</v>
+        <v>461</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A203" s="6" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A204" s="6" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A205" s="6" t="s">
-        <v>217</v>
+        <v>462</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A206" s="6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A207" s="6" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A208" s="6" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A209" s="6" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A210" s="6" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A211" s="6" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A212" s="6" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A213" s="6" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A214" s="6" t="s">
-        <v>463</v>
+        <v>225</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A215" s="6" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A216" s="6" t="s">
-        <v>464</v>
+        <v>227</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A217" s="6" t="s">
-        <v>465</v>
+        <v>228</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A218" s="6" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A219" s="6" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A220" s="6" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A221" s="6" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A222" s="6" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A223" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A224" s="6" t="s">
-        <v>248</v>
+        <v>467</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A225" s="6" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A226" s="6" t="s">
-        <v>251</v>
+        <v>469</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A227" s="6" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A228" s="6" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A229" s="6" t="s">
-        <v>259</v>
+        <v>470</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A230" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A231" s="6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A232" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A233" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A234" s="6" t="s">
         <v>471</v>
       </c>
     </row>
@@ -4146,8 +4233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B14C633B-6035-1E43-B90D-3AAF5179DC67}">
   <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4218,8 +4305,8 @@
       <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
+      <c r="J2" s="1">
+        <v>0</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>14</v>
@@ -4253,8 +4340,8 @@
       <c r="I3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>14</v>
+      <c r="J3" s="1">
+        <v>0</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>14</v>
@@ -4288,8 +4375,8 @@
       <c r="I4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>14</v>
+      <c r="J4" s="1">
+        <v>0</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>14</v>
@@ -4323,8 +4410,8 @@
       <c r="I5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>14</v>
+      <c r="J5" s="1">
+        <v>0</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>14</v>
@@ -4428,8 +4515,8 @@
       <c r="I8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>14</v>
+      <c r="J8" s="1">
+        <v>0</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>14</v>
@@ -4463,8 +4550,8 @@
       <c r="I9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>14</v>
+      <c r="J9" s="1">
+        <v>0</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>14</v>
@@ -4498,8 +4585,8 @@
       <c r="I10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>14</v>
+      <c r="J10" s="1">
+        <v>0</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>14</v>
@@ -4533,8 +4620,8 @@
       <c r="I11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>14</v>
+      <c r="J11" s="1">
+        <v>0</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>14</v>
@@ -4568,8 +4655,8 @@
       <c r="I12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>14</v>
+      <c r="J12" s="1">
+        <v>0</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>14</v>
@@ -4603,8 +4690,8 @@
       <c r="I13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>14</v>
+      <c r="J13" s="1">
+        <v>0</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>14</v>
@@ -4638,8 +4725,8 @@
       <c r="I14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>14</v>
+      <c r="J14" s="1">
+        <v>0</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>14</v>
@@ -4673,8 +4760,8 @@
       <c r="I15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>14</v>
+      <c r="J15" s="1">
+        <v>0</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>14</v>
@@ -4708,8 +4795,8 @@
       <c r="I16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>14</v>
+      <c r="J16" s="1">
+        <v>0</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>14</v>
@@ -4743,8 +4830,8 @@
       <c r="I17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>14</v>
+      <c r="J17" s="1">
+        <v>0</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>14</v>
@@ -4778,8 +4865,8 @@
       <c r="I18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>14</v>
+      <c r="J18" s="1">
+        <v>0</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>14</v>
@@ -4813,8 +4900,8 @@
       <c r="I19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>14</v>
+      <c r="J19" s="1">
+        <v>0</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>14</v>
@@ -4848,8 +4935,8 @@
       <c r="I20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>14</v>
+      <c r="J20" s="1">
+        <v>0</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>14</v>
@@ -4883,8 +4970,8 @@
       <c r="I21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>14</v>
+      <c r="J21" s="1">
+        <v>0</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>14</v>
@@ -4918,8 +5005,8 @@
       <c r="I22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J22" s="1" t="s">
-        <v>14</v>
+      <c r="J22" s="1">
+        <v>0</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>14</v>
@@ -4953,8 +5040,8 @@
       <c r="I23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>14</v>
+      <c r="J23" s="1">
+        <v>0</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>14</v>
@@ -5058,8 +5145,8 @@
       <c r="I26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>14</v>
+      <c r="J26" s="1">
+        <v>0</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>14</v>
@@ -5093,8 +5180,8 @@
       <c r="I27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>14</v>
+      <c r="J27" s="1">
+        <v>0</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>14</v>
@@ -5163,8 +5250,8 @@
       <c r="I29" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J29" s="1" t="s">
-        <v>14</v>
+      <c r="J29" s="1">
+        <v>0</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>14</v>
@@ -5233,8 +5320,8 @@
       <c r="I31" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J31" s="1" t="s">
-        <v>14</v>
+      <c r="J31" s="1">
+        <v>0</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>14</v>
@@ -5373,8 +5460,8 @@
       <c r="I35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>14</v>
+      <c r="J35" s="1">
+        <v>0</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>14</v>
@@ -5408,8 +5495,8 @@
       <c r="I36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J36" s="1" t="s">
-        <v>14</v>
+      <c r="J36" s="1">
+        <v>0</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>14</v>
@@ -5443,8 +5530,8 @@
       <c r="I37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J37" s="1" t="s">
-        <v>14</v>
+      <c r="J37" s="1">
+        <v>0</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>14</v>
@@ -5478,8 +5565,8 @@
       <c r="I38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J38" s="1" t="s">
-        <v>14</v>
+      <c r="J38" s="1">
+        <v>0</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>14</v>
@@ -5513,8 +5600,8 @@
       <c r="I39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>14</v>
+      <c r="J39" s="1">
+        <v>0</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>14</v>
@@ -5583,8 +5670,8 @@
       <c r="I41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J41" s="1" t="s">
-        <v>14</v>
+      <c r="J41" s="1">
+        <v>0</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>14</v>
@@ -5618,8 +5705,8 @@
       <c r="I42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J42" s="1" t="s">
-        <v>14</v>
+      <c r="J42" s="1">
+        <v>0</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>14</v>
@@ -5653,8 +5740,8 @@
       <c r="I43" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J43" s="1" t="s">
-        <v>14</v>
+      <c r="J43" s="1">
+        <v>0</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>14</v>
@@ -5688,8 +5775,8 @@
       <c r="I44" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J44" s="1" t="s">
-        <v>14</v>
+      <c r="J44" s="1">
+        <v>0</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>14</v>
@@ -5723,8 +5810,8 @@
       <c r="I45" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J45" s="1" t="s">
-        <v>14</v>
+      <c r="J45" s="1">
+        <v>0</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>14</v>
@@ -5758,8 +5845,8 @@
       <c r="I46" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J46" s="1" t="s">
-        <v>14</v>
+      <c r="J46" s="1">
+        <v>0</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>14</v>
@@ -5793,8 +5880,8 @@
       <c r="I47" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J47" s="1" t="s">
-        <v>14</v>
+      <c r="J47" s="1">
+        <v>0</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>14</v>
@@ -5828,8 +5915,8 @@
       <c r="I48" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J48" s="1" t="s">
-        <v>14</v>
+      <c r="J48" s="1">
+        <v>0</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>14</v>
@@ -6003,8 +6090,8 @@
       <c r="I53" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J53" s="1" t="s">
-        <v>14</v>
+      <c r="J53" s="1">
+        <v>0</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>14</v>
@@ -6073,8 +6160,8 @@
       <c r="I55" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J55" s="1" t="s">
-        <v>14</v>
+      <c r="J55" s="1">
+        <v>0</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>14</v>
@@ -6108,8 +6195,8 @@
       <c r="I56" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J56" s="1" t="s">
-        <v>14</v>
+      <c r="J56" s="1">
+        <v>0</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>14</v>
@@ -6143,8 +6230,8 @@
       <c r="I57" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J57" s="1" t="s">
-        <v>14</v>
+      <c r="J57" s="1">
+        <v>0</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>14</v>
@@ -6178,8 +6265,8 @@
       <c r="I58" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J58" s="1" t="s">
-        <v>14</v>
+      <c r="J58" s="1">
+        <v>0</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>14</v>
@@ -6213,8 +6300,8 @@
       <c r="I59" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J59" s="1" t="s">
-        <v>14</v>
+      <c r="J59" s="1">
+        <v>0</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>14</v>
@@ -6283,8 +6370,8 @@
       <c r="I61" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J61" s="1" t="s">
-        <v>14</v>
+      <c r="J61" s="1">
+        <v>0</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>14</v>
@@ -6318,8 +6405,8 @@
       <c r="I62" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J62" s="1" t="s">
-        <v>14</v>
+      <c r="J62" s="1">
+        <v>0</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>14</v>
@@ -6353,8 +6440,8 @@
       <c r="I63" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J63" s="1" t="s">
-        <v>14</v>
+      <c r="J63" s="1">
+        <v>0</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>14</v>
@@ -6528,8 +6615,8 @@
       <c r="I68" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J68" s="1" t="s">
-        <v>14</v>
+      <c r="J68" s="1">
+        <v>0</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>14</v>
@@ -6563,8 +6650,8 @@
       <c r="I69" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J69" s="1" t="s">
-        <v>14</v>
+      <c r="J69" s="1">
+        <v>0</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>14</v>
@@ -6633,8 +6720,8 @@
       <c r="I71" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J71" s="1" t="s">
-        <v>14</v>
+      <c r="J71" s="1">
+        <v>0</v>
       </c>
       <c r="K71" s="1" t="s">
         <v>14</v>
@@ -6668,8 +6755,8 @@
       <c r="I72" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J72" s="1" t="s">
-        <v>14</v>
+      <c r="J72" s="1">
+        <v>0</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>14</v>
@@ -6703,8 +6790,8 @@
       <c r="I73" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J73" s="1" t="s">
-        <v>14</v>
+      <c r="J73" s="1">
+        <v>0</v>
       </c>
       <c r="K73" s="1" t="s">
         <v>14</v>
@@ -6738,8 +6825,8 @@
       <c r="I74" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J74" s="1" t="s">
-        <v>14</v>
+      <c r="J74" s="1">
+        <v>0</v>
       </c>
       <c r="K74" s="1" t="s">
         <v>14</v>
@@ -6773,8 +6860,8 @@
       <c r="I75" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J75" s="1" t="s">
-        <v>14</v>
+      <c r="J75" s="1">
+        <v>0</v>
       </c>
       <c r="K75" s="1" t="s">
         <v>14</v>
@@ -6843,8 +6930,8 @@
       <c r="I77" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J77" s="1" t="s">
-        <v>14</v>
+      <c r="J77" s="1">
+        <v>0</v>
       </c>
       <c r="K77" s="1" t="s">
         <v>14</v>
@@ -6948,8 +7035,8 @@
       <c r="I80" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J80" s="1" t="s">
-        <v>14</v>
+      <c r="J80" s="1">
+        <v>0</v>
       </c>
       <c r="K80" s="1" t="s">
         <v>14</v>
@@ -6983,8 +7070,8 @@
       <c r="I81" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J81" s="1" t="s">
-        <v>14</v>
+      <c r="J81" s="1">
+        <v>0</v>
       </c>
       <c r="K81" s="1" t="s">
         <v>14</v>
@@ -7018,8 +7105,8 @@
       <c r="I82" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J82" s="1" t="s">
-        <v>14</v>
+      <c r="J82" s="1">
+        <v>0</v>
       </c>
       <c r="K82" s="1" t="s">
         <v>14</v>
@@ -7053,8 +7140,8 @@
       <c r="I83" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J83" s="1" t="s">
-        <v>14</v>
+      <c r="J83" s="1">
+        <v>0</v>
       </c>
       <c r="K83" s="1" t="s">
         <v>14</v>
@@ -7088,8 +7175,8 @@
       <c r="I84" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J84" s="1" t="s">
-        <v>14</v>
+      <c r="J84" s="1">
+        <v>0</v>
       </c>
       <c r="K84" s="1" t="s">
         <v>14</v>
@@ -7123,8 +7210,8 @@
       <c r="I85" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J85" s="1" t="s">
-        <v>14</v>
+      <c r="J85" s="1">
+        <v>0</v>
       </c>
       <c r="K85" s="1" t="s">
         <v>14</v>
@@ -7158,8 +7245,8 @@
       <c r="I86" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J86" s="1" t="s">
-        <v>14</v>
+      <c r="J86" s="1">
+        <v>0</v>
       </c>
       <c r="K86" s="1" t="s">
         <v>14</v>
@@ -7193,8 +7280,8 @@
       <c r="I87" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J87" s="1" t="s">
-        <v>14</v>
+      <c r="J87" s="1">
+        <v>0</v>
       </c>
       <c r="K87" s="1" t="s">
         <v>14</v>
@@ -7228,8 +7315,8 @@
       <c r="I88" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J88" s="1" t="s">
-        <v>14</v>
+      <c r="J88" s="1">
+        <v>0</v>
       </c>
       <c r="K88" s="1" t="s">
         <v>14</v>
@@ -7263,8 +7350,8 @@
       <c r="I89" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J89" s="1" t="s">
-        <v>14</v>
+      <c r="J89" s="1">
+        <v>0</v>
       </c>
       <c r="K89" s="1" t="s">
         <v>14</v>
@@ -7298,8 +7385,8 @@
       <c r="I90" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J90" s="1" t="s">
-        <v>14</v>
+      <c r="J90" s="1">
+        <v>0</v>
       </c>
       <c r="K90" s="1" t="s">
         <v>14</v>
@@ -7333,8 +7420,8 @@
       <c r="I91" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J91" s="1" t="s">
-        <v>14</v>
+      <c r="J91" s="1">
+        <v>0</v>
       </c>
       <c r="K91" s="1" t="s">
         <v>14</v>
@@ -7368,8 +7455,8 @@
       <c r="I92" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J92" s="1" t="s">
-        <v>14</v>
+      <c r="J92" s="1">
+        <v>0</v>
       </c>
       <c r="K92" s="1" t="s">
         <v>14</v>
@@ -7403,8 +7490,8 @@
       <c r="I93" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J93" s="1" t="s">
-        <v>14</v>
+      <c r="J93" s="1">
+        <v>0</v>
       </c>
       <c r="K93" s="1" t="s">
         <v>14</v>
@@ -7438,8 +7525,8 @@
       <c r="I94" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J94" s="1" t="s">
-        <v>14</v>
+      <c r="J94" s="1">
+        <v>0</v>
       </c>
       <c r="K94" s="1" t="s">
         <v>14</v>
@@ -7473,8 +7560,8 @@
       <c r="I95" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J95" s="1" t="s">
-        <v>14</v>
+      <c r="J95" s="1">
+        <v>0</v>
       </c>
       <c r="K95" s="1" t="s">
         <v>14</v>
@@ -7543,8 +7630,8 @@
       <c r="I97" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J97" s="1" t="s">
-        <v>14</v>
+      <c r="J97" s="1">
+        <v>0</v>
       </c>
       <c r="K97" s="1" t="s">
         <v>14</v>
@@ -7578,8 +7665,8 @@
       <c r="I98" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J98" s="1" t="s">
-        <v>14</v>
+      <c r="J98" s="1">
+        <v>0</v>
       </c>
       <c r="K98" s="1" t="s">
         <v>14</v>
@@ -7648,8 +7735,8 @@
       <c r="I100" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J100" s="1" t="s">
-        <v>14</v>
+      <c r="J100" s="1">
+        <v>0</v>
       </c>
       <c r="K100" s="1" t="s">
         <v>14</v>
@@ -7683,8 +7770,8 @@
       <c r="I101" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J101" s="1" t="s">
-        <v>14</v>
+      <c r="J101" s="1">
+        <v>0</v>
       </c>
       <c r="K101" s="1" t="s">
         <v>14</v>
@@ -7718,8 +7805,8 @@
       <c r="I102" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J102" s="1" t="s">
-        <v>14</v>
+      <c r="J102" s="1">
+        <v>0</v>
       </c>
       <c r="K102" s="1" t="s">
         <v>14</v>
@@ -7753,8 +7840,8 @@
       <c r="I103" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J103" s="1" t="s">
-        <v>14</v>
+      <c r="J103" s="1">
+        <v>0</v>
       </c>
       <c r="K103" s="1" t="s">
         <v>14</v>
@@ -7788,8 +7875,8 @@
       <c r="I104" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J104" s="1" t="s">
-        <v>14</v>
+      <c r="J104" s="1">
+        <v>0</v>
       </c>
       <c r="K104" s="1" t="s">
         <v>14</v>
@@ -7823,8 +7910,8 @@
       <c r="I105" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J105" s="1" t="s">
-        <v>14</v>
+      <c r="J105" s="1">
+        <v>0</v>
       </c>
       <c r="K105" s="1" t="s">
         <v>14</v>
@@ -7858,8 +7945,8 @@
       <c r="I106" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J106" s="1" t="s">
-        <v>14</v>
+      <c r="J106" s="1">
+        <v>0</v>
       </c>
       <c r="K106" s="1" t="s">
         <v>14</v>
@@ -7963,8 +8050,8 @@
       <c r="I109" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J109" s="1" t="s">
-        <v>14</v>
+      <c r="J109" s="1">
+        <v>0</v>
       </c>
       <c r="K109" s="1" t="s">
         <v>14</v>
@@ -7998,8 +8085,8 @@
       <c r="I110" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J110" s="1" t="s">
-        <v>14</v>
+      <c r="J110" s="1">
+        <v>0</v>
       </c>
       <c r="K110" s="1" t="s">
         <v>14</v>
@@ -8033,8 +8120,8 @@
       <c r="I111" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J111" s="1" t="s">
-        <v>14</v>
+      <c r="J111" s="1">
+        <v>0</v>
       </c>
       <c r="K111" s="1" t="s">
         <v>14</v>
@@ -8173,8 +8260,8 @@
       <c r="I115" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J115" s="1" t="s">
-        <v>14</v>
+      <c r="J115" s="1">
+        <v>0</v>
       </c>
       <c r="K115" s="1" t="s">
         <v>14</v>
@@ -8278,8 +8365,8 @@
       <c r="I118" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J118" s="1" t="s">
-        <v>14</v>
+      <c r="J118" s="1">
+        <v>0</v>
       </c>
       <c r="K118" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
rerun count and cover
</commit_message>
<xml_diff>
--- a/00_Data/Master_files/plant_info_MASTER.xlsx
+++ b/00_Data/Master_files/plant_info_MASTER.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="5" r:id="rId1"/>
     <sheet name="PROJECT_METADATA" sheetId="2" r:id="rId2"/>
     <sheet name="plant_info" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="566">
   <si>
     <t>Species</t>
   </si>
@@ -1796,9 +1796,6 @@
   </si>
   <si>
     <t>Era_sp. - Eragrostis sp. (Tall ALG), so they’re both different, but only native has , so we can delete Eran_sp. and just use Era_sp.</t>
-  </si>
-  <si>
-    <t>COVER DATA NOTES:</t>
   </si>
 </sst>
 </file>
@@ -2729,8 +2726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:A59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2959,9 +2956,7 @@
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
-        <v>566</v>
-      </c>
+      <c r="A59" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4321,8 +4316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -8427,10 +8422,10 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>11</v>
@@ -8448,13 +8443,13 @@
         <v>5</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="I118" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J118" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K118" s="1" t="s">
         <v>14</v>
@@ -8462,10 +8457,10 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>11</v>
@@ -8483,13 +8478,13 @@
         <v>5</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I119" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J119" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K119" s="1" t="s">
         <v>14</v>

</xml_diff>